<commit_message>
Standardize schema to snake_case and generate camelCase for TypeScript
</commit_message>
<xml_diff>
--- a/project/excel/oct_schema.xlsx
+++ b/project/excel/oct_schema.xlsx
@@ -443,22 +443,22 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>siteTypeIds</t>
+          <t>site_type_ids</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>speciesIds</t>
+          <t>species_ids</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>urlPath</t>
+          <t>url_path</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>internalPath</t>
+          <t>internal_path</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -473,27 +473,27 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>createdAt</t>
+          <t>created_at</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>createdById</t>
+          <t>created_by_id</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>updatedAt</t>
+          <t>updated_at</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>updatedById</t>
+          <t>updated_by_id</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>organizationId</t>
+          <t>organization_id</t>
         </is>
       </c>
     </row>
@@ -508,7 +508,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,27 +519,52 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>org_id</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>created_at</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>updated_at</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>country</t>
-        </is>
-      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>metadata</t>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>region</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>website_url</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>contact_email</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>logo_url</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>is_active</t>
         </is>
       </c>
     </row>
@@ -565,7 +590,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>siteTypeId</t>
+          <t>site_type_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -575,7 +600,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>groupIdHierarchy</t>
+          <t>group_id_hierarchy</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -585,12 +610,12 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>urlPath</t>
+          <t>url_path</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>internalPath</t>
+          <t>internal_path</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -605,27 +630,27 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>createdAt</t>
+          <t>created_at</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>createdById</t>
+          <t>created_by_id</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>updatedAt</t>
+          <t>updated_at</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>updatedById</t>
+          <t>updated_by_id</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>organizationId</t>
+          <t>organization_id</t>
         </is>
       </c>
     </row>
@@ -651,7 +676,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>groupTypeId</t>
+          <t>group_type_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -661,12 +686,12 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>siteId</t>
+          <t>site_id</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>parentId</t>
+          <t>parent_id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -681,12 +706,12 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>urlPath</t>
+          <t>url_path</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>internalPath</t>
+          <t>internal_path</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
@@ -701,27 +726,27 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>createdAt</t>
+          <t>created_at</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>createdById</t>
+          <t>created_by_id</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>updatedAt</t>
+          <t>updated_at</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>updatedById</t>
+          <t>updated_by_id</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>organizationId</t>
+          <t>organization_id</t>
         </is>
       </c>
     </row>
@@ -752,37 +777,37 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>speciesId</t>
+          <t>species_id</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>genetTypeId</t>
+          <t>genet_type_id</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>sfId</t>
+          <t>sf_id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>clonalId</t>
+          <t>clonal_id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>accessionNumber</t>
+          <t>accession_number</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>urlPath</t>
+          <t>url_path</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>internalPath</t>
+          <t>internal_path</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
@@ -797,27 +822,27 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>createdAt</t>
+          <t>created_at</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>createdById</t>
+          <t>created_by_id</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>updatedAt</t>
+          <t>updated_at</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>updatedById</t>
+          <t>updated_by_id</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>organizationId</t>
+          <t>organization_id</t>
         </is>
       </c>
     </row>
@@ -848,27 +873,27 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>genetId</t>
+          <t>genet_id</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>speciesId</t>
+          <t>species_id</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>siteId</t>
+          <t>site_id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>groupId</t>
+          <t>group_id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>coralTypeId</t>
+          <t>coral_type_id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -883,12 +908,12 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>urlPath</t>
+          <t>url_path</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>internalPath</t>
+          <t>internal_path</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
@@ -903,27 +928,27 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>createdAt</t>
+          <t>created_at</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>createdById</t>
+          <t>created_by_id</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>updatedAt</t>
+          <t>updated_at</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>updatedById</t>
+          <t>updated_by_id</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>organizationId</t>
+          <t>organization_id</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1030,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>imageUrl</t>
+          <t>image_url</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -1015,27 +1040,27 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>createdAt</t>
+          <t>created_at</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>createdById</t>
+          <t>created_by_id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>updatedAt</t>
+          <t>updated_at</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>updatedById</t>
+          <t>updated_by_id</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>organizationId</t>
+          <t>organization_id</t>
         </is>
       </c>
     </row>
@@ -1061,27 +1086,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>eventTypeId</t>
+          <t>event_type_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>recordId</t>
+          <t>record_id</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>recordModelType</t>
+          <t>record_model_type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>urlPath</t>
+          <t>url_path</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>internalPath</t>
+          <t>internal_path</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -1096,27 +1121,27 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>createdAt</t>
+          <t>created_at</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>createdById</t>
+          <t>created_by_id</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>updatedAt</t>
+          <t>updated_at</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>updatedById</t>
+          <t>updated_by_id</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>organizationId</t>
+          <t>organization_id</t>
         </is>
       </c>
     </row>
@@ -1136,7 +1161,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1147,42 +1172,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>code</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>created_at</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>updated_at</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>common_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>genus</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>specific_epithet</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>scientific_name</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>scientific_name_authorship</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>external_references</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>synonyms</t>
-        </is>
-      </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>deprecated_codes</t>
+          <t>photo_url</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>tags</t>
         </is>
       </c>
     </row>

</xml_diff>